<commit_message>
Completed code and plotting for VT 1.
</commit_message>
<xml_diff>
--- a/DHW.xlsx
+++ b/DHW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EDAEE9-F685-44CB-A3D4-77C7EA86FEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E147C11-3350-437C-AA36-F850D5926A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9615D349-3226-4407-857B-2CC3135C9C54}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Appliances" sheetId="1" r:id="rId1"/>
     <sheet name="Usage Pattern" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -421,11 +421,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -509,6 +524,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -828,69 +858,69 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="17">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="17">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="17">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="33">
         <v>10</v>
       </c>
     </row>
@@ -903,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC79B40B-C856-4E54-8710-0EF3281988E2}">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="12">
         <v>0</v>
@@ -1229,13 +1259,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="12">
         <v>0</v>
       </c>
       <c r="Q4" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="11">
         <v>1</v>
@@ -1244,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="12">
         <v>0</v>
@@ -1259,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="12">
         <v>0</v>
@@ -1271,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="AC4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="12">
         <v>0</v>
@@ -1286,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="AH4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="12">
         <v>0</v>
@@ -1346,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="15">
         <v>0</v>
@@ -1421,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="20">
         <v>0</v>
@@ -1436,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="20">
         <v>0</v>
@@ -1445,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="19">
         <v>0</v>
@@ -1457,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="19">
         <v>0</v>
@@ -1475,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="19">
         <v>0</v>
@@ -1505,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="AG6" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="19">
         <v>0</v>
       </c>
       <c r="AI6" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" s="20">
         <v>0</v>
@@ -1541,13 +1571,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="15">
         <v>0</v>
       </c>
       <c r="J7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="16">
         <v>0</v>
@@ -1556,28 +1586,28 @@
         <v>0</v>
       </c>
       <c r="M7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="15">
         <v>0</v>
       </c>
       <c r="O7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="16">
         <v>0</v>
       </c>
       <c r="Q7" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="15">
         <v>0</v>
       </c>
       <c r="T7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="16">
         <v>0</v>
@@ -1586,13 +1616,13 @@
         <v>0</v>
       </c>
       <c r="W7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="15">
         <v>0</v>
       </c>
       <c r="Y7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="16">
         <v>0</v>
@@ -1601,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="AB7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" s="15">
         <v>0</v>
       </c>
       <c r="AD7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7" s="16">
         <v>0</v>
@@ -1616,13 +1646,13 @@
         <v>0</v>
       </c>
       <c r="AG7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7" s="15">
         <v>0</v>
       </c>
       <c r="AI7" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7" s="16">
         <v>0</v>
@@ -1637,106 +1667,106 @@
         <v>0</v>
       </c>
       <c r="C8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="18">
         <v>0</v>
       </c>
       <c r="H8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="18">
         <v>0</v>
       </c>
       <c r="M8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="18">
         <v>0</v>
       </c>
       <c r="W8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="18">
         <v>0</v>
       </c>
       <c r="AB8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="18">
         <v>0</v>
       </c>
       <c r="AG8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1748,58 +1778,58 @@
         <v>0</v>
       </c>
       <c r="C9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="14">
         <v>0</v>
       </c>
       <c r="H9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="14">
         <v>0</v>
       </c>
       <c r="M9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="16">
         <v>0</v>
       </c>
       <c r="Q9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="16">
         <v>0</v>
@@ -1808,13 +1838,13 @@
         <v>0</v>
       </c>
       <c r="W9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="16">
         <v>0</v>
@@ -1823,31 +1853,31 @@
         <v>0</v>
       </c>
       <c r="AB9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="14">
         <v>0</v>
       </c>
       <c r="AG9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>